<commit_message>
complete add recipie method
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Hypothyroidism.xlsx
+++ b/src/test/resources/output/Hypothyroidism.xlsx
@@ -6,13 +6,14 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hypothyroidism" r:id="rId3" sheetId="1"/>
+    <sheet name="HypothyroidismAdd" r:id="rId3" sheetId="1"/>
+    <sheet name="HypothyroidismEliminate" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="338">
   <si>
     <t>Recipe ID</t>
   </si>
@@ -50,7 +51,7 @@
     <t>Masala Chawli</t>
   </si>
   <si>
-    <t xml:space="preserve">1/2 cup chawli (cow pea / lobhia) , soaked overnight and drained    salt to taste    1 tbsp coconut oil or oil    1/2 cup finely chopped onions    1 cup fresh tomato pulp    1/2 tsp dried fenugreek leaves (kasuri methi)    1/4 tsp turmeric powder (haldi)    3/4 cup chopped mint leaves (phudina) , washed and drained    1 tsp roughly chopped ginger (adrak)    2 tsp roughly chopped green chillies    1/2 tsp lemon juice    </t>
+    <t xml:space="preserve">1/2 cup chawli (cow pea / lobhia) , soaked overnight and drained    salt to taste    </t>
   </si>
   <si>
     <t>15 mins</t>
@@ -83,6 +84,45 @@
   </si>
   <si>
     <t>https://www.tarladalal.com/masala-chawli-3883r</t>
+  </si>
+  <si>
+    <t>Recipe# 40603</t>
+  </si>
+  <si>
+    <t>Baingan Bhaja, Bengali Begun Bhaja</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>10 mins</t>
+  </si>
+  <si>
+    <t>20 mins</t>
+  </si>
+  <si>
+    <t>, For baingan bhaja
+To make baingan bhaja, combine the chilli powder, turmeric powder, lemon juice, besan, salt and 2 tbsp of water in a deep bowl and mix well.
+Add the baingan slices and mix well. Keep aside.
+Heat a non-stick tava (griddle), grease it with ½ tsp of oil, arrange half the baingan slices and cook using ½ tsp of oil on both the sides till golden brown in colour.
+Repeat step 3 to make 1 more batch.
+Serve the baingan bhaja immediately.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per serving
+Energy 43 cal
+Protein 1.5 g
+Carbohydrates 4.6 g
+Fiber 3 g
+Fat 2.1 g
+Cholesterol 0 mg
+Sodium 4.3 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/baingan-bhaja-bengali-begun-bhaja-40603r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2 cup chawli (cow pea / lobhia) , soaked overnight and drained    salt to taste    1 tbsp coconut oil or oil    1/2 cup finely chopped onions    1 cup fresh tomato pulp    1/2 tsp dried fenugreek leaves (kasuri methi)    1/4 tsp turmeric powder (haldi)    3/4 cup chopped mint leaves (phudina) , washed and drained    1 tsp roughly chopped ginger (adrak)    2 tsp roughly chopped green chillies    1/2 tsp lemon juice    </t>
   </si>
   <si>
     <t>Recipe# 3577</t>
@@ -158,40 +198,7 @@
     <t>https://www.tarladalal.com/chana-tuvar-and-green-moong-dal-trevati-dal-38470r</t>
   </si>
   <si>
-    <t>Recipe# 40603</t>
-  </si>
-  <si>
-    <t>Baingan Bhaja, Bengali Begun Bhaja</t>
-  </si>
-  <si>
     <t xml:space="preserve">18 big brinjal (baingan / eggplant) slices    2 tsp chilli powder    1/2 tsp turmeric powder (haldi)    1 tbsp lemon juice    1/4 cup besan (bengal gram flour)    salt to taste    2 tsp oil for greasing and cooking    </t>
-  </si>
-  <si>
-    <t>10 mins</t>
-  </si>
-  <si>
-    <t>20 mins</t>
-  </si>
-  <si>
-    <t>, For baingan bhaja
-To make baingan bhaja, combine the chilli powder, turmeric powder, lemon juice, besan, salt and 2 tbsp of water in a deep bowl and mix well.
-Add the baingan slices and mix well. Keep aside.
-Heat a non-stick tava (griddle), grease it with ½ tsp of oil, arrange half the baingan slices and cook using ½ tsp of oil on both the sides till golden brown in colour.
-Repeat step 3 to make 1 more batch.
-Serve the baingan bhaja immediately.</t>
-  </si>
-  <si>
-    <t>Nutrient values (Abbrv) per serving
-Energy 43 cal
-Protein 1.5 g
-Carbohydrates 4.6 g
-Fiber 3 g
-Fat 2.1 g
-Cholesterol 0 mg
-Sodium 4.3 mg</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/baingan-bhaja-bengali-begun-bhaja-40603r</t>
   </si>
   <si>
     <t>Recipe# 5292</t>
@@ -1690,7 +1697,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1798,12 +1805,127 @@
         <v>26</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:K52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>2</v>
@@ -1812,33 +1934,33 @@
         <v>3</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>2</v>
@@ -1847,33 +1969,33 @@
         <v>3</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="J5" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K5" t="s" s="0">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>2</v>
@@ -1882,33 +2004,33 @@
         <v>3</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J6" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K6" t="s" s="0">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>2</v>
@@ -1917,33 +2039,33 @@
         <v>3</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s" s="0">
         <v>13</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J7" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K7" t="s" s="0">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>2</v>
@@ -1952,33 +2074,33 @@
         <v>3</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J8" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K8" t="s" s="0">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>2</v>
@@ -1987,33 +2109,33 @@
         <v>3</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F9" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J9" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K9" t="s" s="0">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>2</v>
@@ -2022,33 +2144,33 @@
         <v>3</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="H10" t="s" s="0">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J10" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K10" t="s" s="0">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>2</v>
@@ -2057,33 +2179,33 @@
         <v>3</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H11" t="s" s="0">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I11" t="s" s="0">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J11" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K11" t="s" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s" s="0">
         <v>2</v>
@@ -2092,33 +2214,33 @@
         <v>3</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F12" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G12" t="s" s="0">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="H12" t="s" s="0">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I12" t="s" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J12" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K12" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s" s="0">
         <v>2</v>
@@ -2127,33 +2249,33 @@
         <v>3</v>
       </c>
       <c r="E13" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F13" t="s" s="0">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="G13" t="s" s="0">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="H13" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I13" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J13" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K13" t="s" s="0">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s" s="0">
         <v>2</v>
@@ -2162,33 +2284,33 @@
         <v>3</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F14" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G14" t="s" s="0">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H14" t="s" s="0">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I14" t="s" s="0">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J14" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K14" t="s" s="0">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s" s="0">
         <v>2</v>
@@ -2197,33 +2319,33 @@
         <v>3</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F15" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G15" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H15" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I15" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J15" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K15" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C16" t="s" s="0">
         <v>2</v>
@@ -2232,33 +2354,33 @@
         <v>3</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F16" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H16" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I16" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J16" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s" s="0">
         <v>2</v>
@@ -2267,33 +2389,33 @@
         <v>3</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F17" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G17" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H17" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I17" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J17" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K17" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>2</v>
@@ -2302,33 +2424,33 @@
         <v>3</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F18" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G18" t="s" s="0">
         <v>13</v>
       </c>
       <c r="H18" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I18" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J18" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K18" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>2</v>
@@ -2337,33 +2459,33 @@
         <v>3</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F19" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G19" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H19" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I19" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="J19" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K19" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C20" t="s" s="0">
         <v>2</v>
@@ -2372,33 +2494,33 @@
         <v>3</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F20" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G20" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H20" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I20" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="J20" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K20" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C21" t="s" s="0">
         <v>2</v>
@@ -2407,33 +2529,33 @@
         <v>3</v>
       </c>
       <c r="E21" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F21" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G21" t="s" s="0">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="H21" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="I21" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="J21" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K21" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C22" t="s" s="0">
         <v>2</v>
@@ -2442,33 +2564,33 @@
         <v>3</v>
       </c>
       <c r="E22" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F22" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G22" t="s" s="0">
         <v>13</v>
       </c>
       <c r="H22" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="I22" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="J22" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K22" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C23" t="s" s="0">
         <v>2</v>
@@ -2477,33 +2599,33 @@
         <v>3</v>
       </c>
       <c r="E23" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F23" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G23" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H23" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="I23" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="J23" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K23" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C24" t="s" s="0">
         <v>2</v>
@@ -2512,33 +2634,33 @@
         <v>3</v>
       </c>
       <c r="E24" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G24" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H24" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I24" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J24" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K24" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C25" t="s" s="0">
         <v>2</v>
@@ -2547,33 +2669,33 @@
         <v>3</v>
       </c>
       <c r="E25" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F25" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G25" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H25" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="I25" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="J25" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K25" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C26" t="s" s="0">
         <v>2</v>
@@ -2582,33 +2704,33 @@
         <v>3</v>
       </c>
       <c r="E26" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F26" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G26" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H26" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="I26" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="J26" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K26" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C27" t="s" s="0">
         <v>2</v>
@@ -2617,33 +2739,33 @@
         <v>3</v>
       </c>
       <c r="E27" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F27" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G27" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="H27" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I27" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="J27" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K27" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C28" t="s" s="0">
         <v>2</v>
@@ -2652,7 +2774,7 @@
         <v>3</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F28" t="s" s="0">
         <v>13</v>
@@ -2661,24 +2783,24 @@
         <v>13</v>
       </c>
       <c r="H28" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="I28" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="J28" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K28" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C29" t="s" s="0">
         <v>2</v>
@@ -2687,33 +2809,33 @@
         <v>3</v>
       </c>
       <c r="E29" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F29" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G29" t="s" s="0">
         <v>13</v>
       </c>
       <c r="H29" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="I29" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="J29" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K29" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C30" t="s" s="0">
         <v>2</v>
@@ -2722,33 +2844,33 @@
         <v>3</v>
       </c>
       <c r="E30" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F30" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G30" t="s" s="0">
         <v>13</v>
       </c>
       <c r="H30" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="I30" t="s" s="0">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="J30" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K30" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C31" t="s" s="0">
         <v>2</v>
@@ -2757,33 +2879,33 @@
         <v>3</v>
       </c>
       <c r="E31" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="F31" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G31" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H31" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="I31" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="J31" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K31" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C32" t="s" s="0">
         <v>2</v>
@@ -2792,33 +2914,33 @@
         <v>3</v>
       </c>
       <c r="E32" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="F32" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G32" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="H32" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="J32" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K32" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C33" t="s" s="0">
         <v>2</v>
@@ -2827,33 +2949,33 @@
         <v>3</v>
       </c>
       <c r="E33" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F33" t="s" s="0">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="G33" t="s" s="0">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H33" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="I33" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="J33" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K33" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C34" t="s" s="0">
         <v>2</v>
@@ -2862,33 +2984,33 @@
         <v>3</v>
       </c>
       <c r="E34" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F34" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G34" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H34" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="I34" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="J34" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K34" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C35" t="s" s="0">
         <v>2</v>
@@ -2897,33 +3019,33 @@
         <v>3</v>
       </c>
       <c r="E35" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="F35" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G35" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H35" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="I35" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="J35" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K35" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C36" t="s" s="0">
         <v>2</v>
@@ -2932,33 +3054,33 @@
         <v>3</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F36" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G36" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="H36" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="I36" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="J36" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K36" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C37" t="s" s="0">
         <v>2</v>
@@ -2967,33 +3089,33 @@
         <v>3</v>
       </c>
       <c r="E37" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F37" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G37" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H37" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="I37" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="J37" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K37" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C38" t="s" s="0">
         <v>2</v>
@@ -3002,33 +3124,33 @@
         <v>3</v>
       </c>
       <c r="E38" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F38" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G38" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H38" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="I38" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="J38" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K38" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C39" t="s" s="0">
         <v>2</v>
@@ -3037,33 +3159,33 @@
         <v>3</v>
       </c>
       <c r="E39" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="F39" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G39" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H39" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="I39" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J39" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K39" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C40" t="s" s="0">
         <v>2</v>
@@ -3072,33 +3194,33 @@
         <v>3</v>
       </c>
       <c r="E40" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F40" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G40" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H40" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="I40" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="J40" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K40" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C41" t="s" s="0">
         <v>2</v>
@@ -3107,33 +3229,33 @@
         <v>3</v>
       </c>
       <c r="E41" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="F41" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G41" t="s" s="0">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H41" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="I41" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J41" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K41" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C42" t="s" s="0">
         <v>2</v>
@@ -3142,33 +3264,33 @@
         <v>3</v>
       </c>
       <c r="E42" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="F42" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G42" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="H42" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I42" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="J42" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K42" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C43" t="s" s="0">
         <v>2</v>
@@ -3177,33 +3299,33 @@
         <v>3</v>
       </c>
       <c r="E43" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="F43" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G43" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="H43" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="I43" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="J43" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K43" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C44" t="s" s="0">
         <v>2</v>
@@ -3212,33 +3334,33 @@
         <v>3</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="F44" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G44" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H44" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="I44" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="J44" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K44" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C45" t="s" s="0">
         <v>2</v>
@@ -3247,33 +3369,33 @@
         <v>3</v>
       </c>
       <c r="E45" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F45" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G45" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="H45" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="I45" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="J45" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K45" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C46" t="s" s="0">
         <v>2</v>
@@ -3282,33 +3404,33 @@
         <v>3</v>
       </c>
       <c r="E46" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="F46" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G46" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="H46" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="I46" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="J46" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K46" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C47" t="s" s="0">
         <v>2</v>
@@ -3317,33 +3439,33 @@
         <v>3</v>
       </c>
       <c r="E47" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="F47" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G47" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H47" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="I47" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="J47" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K47" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C48" t="s" s="0">
         <v>2</v>
@@ -3352,33 +3474,33 @@
         <v>3</v>
       </c>
       <c r="E48" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="F48" t="s" s="0">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="G48" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H48" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="I48" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="J48" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K48" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C49" t="s" s="0">
         <v>2</v>
@@ -3387,33 +3509,33 @@
         <v>3</v>
       </c>
       <c r="E49" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="F49" t="s" s="0">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G49" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H49" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="I49" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="J49" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K49" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C50" t="s" s="0">
         <v>2</v>
@@ -3422,33 +3544,33 @@
         <v>3</v>
       </c>
       <c r="E50" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="F50" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G50" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H50" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="I50" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="J50" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K50" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C51" t="s" s="0">
         <v>2</v>
@@ -3457,33 +3579,33 @@
         <v>3</v>
       </c>
       <c r="E51" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="F51" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G51" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H51" t="s" s="0">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="I51" t="s" s="0">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="J51" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K51" t="s" s="0">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C52" t="s" s="0">
         <v>2</v>
@@ -3492,25 +3614,25 @@
         <v>3</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="F52" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G52" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H52" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="I52" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="J52" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K52" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit after modification and testing
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Hypothyroidism.xlsx
+++ b/src/test/resources/output/Hypothyroidism.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="353">
   <si>
     <t>Recipe ID</t>
   </si>
@@ -120,6 +120,376 @@
   </si>
   <si>
     <t>https://www.tarladalal.com/baingan-bhaja-bengali-begun-bhaja-40603r</t>
+  </si>
+  <si>
+    <t>Recipe# 42296</t>
+  </si>
+  <si>
+    <t>Quinoa Avocado Veg Healthy Office Salad</t>
+  </si>
+  <si>
+    <t>3 mins</t>
+  </si>
+  <si>
+    <t>, Heat the olive oil in a griller pan or a broad non-stick pan, add the zucchini and sauté on a medium flame for 1 minute.
+Add the coloured capsicum and sauté on a medium flame for 1 minute.
+Add the mushroom and little sea salt and sauté on a medium flame for 1 minute.
+Cool put in a lunch box, along with other ingredients. It can be taken to work with a dressing in a separate small container.
+Just before eating, mix the dressing and toss well. Eat immediately.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per serving
+Energy 459 cal
+Protein 7.7 g
+Carbohydrates 22 g
+Fiber 6.9 g
+Fat 38.9 g
+Cholesterol 0 mg
+Sodium 60.1 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/quinoa-avocado-veg-healthy-office-salad-42296r</t>
+  </si>
+  <si>
+    <t>Recipe# 39929</t>
+  </si>
+  <si>
+    <t>Brown Rice ( Pressure Cooker Method)</t>
+  </si>
+  <si>
+    <t>1 mins</t>
+  </si>
+  <si>
+    <t>, How to cook brown rice
+To cook brown rice, soak the brown rice in enough water for 30 minutes and drain well.
+Combine the brown rice along with 2 cups of water in a pressure cooker and pressure cook for 7 whistles.
+Allow the steam to escape before opening the lid.
+Separate each grain of the brown rice lightly with a fork. Use as required.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per cup
+Energy 211 cal
+Protein 4.4 g
+Carbohydrates 44.4 g
+Fiber 2 g
+Fat 1.6 g
+Cholesterol 0 mg
+Sodium 2.3 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/brown-rice--pressure-cooker-method-39929r</t>
+  </si>
+  <si>
+    <t>Recipe# 42333</t>
+  </si>
+  <si>
+    <t>Egg Paratha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3/4 cup whole wheat flour (gehun ka atta)    1/2 tsp carom seeds (ajwain)    salt to taste    whole wheat flour (gehun ka atta) for rolling    1/2 tsp ghee for spreading    1 tsp oil for cooking    </t>
+  </si>
+  <si>
+    <t>, For the parathas
+Combine all the ingredients in a deep bowl and knead into a soft dough using enough water.
+Divide the dough into 2 equal portions.
+Roll a portion of the dough into 150 mm. (6”) diameter circle using a little whole wheat flour for rolling. Spread ¼ tsp of ghee evenly over it.
+Fold over from one end to another end slightly overlapping each other.
+Then fold again from one end to another end overlapping each other.
+Roll again into a 175 mm. (7”) diameter circle using a little whole wheat flour for rolling.
+Heat a non-stick tava (griddle) and cook the paratha using ½ tsp of oil till it turns golden brown in colour from both the sides
+Repeat steps 3 to 7 to make 1 more paratha. Keep aside.
+For the egg mixture
+Break the eggs in a deep bowl and beat well using a fork.
+Add all the other ingredients and beat well. Keep aside.
+How to proceed
+To make egg paratha, heat a non-stick tava (griddle) and grease it using 1 tsp of oil. Pour half the egg mixture on it.
+Place a prepared paratha on it and press it lightly. Cook using 1 tsp of oil.
+Turnover and cook again till it is cooked.
+Cut into 4 equal portions using a cutter or a sharp knife.
+Repeat steps 1 to 4 to make 1 more egg paratha.
+Serve egg paratha immediately.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per paratha
+Energy 432 cal
+Protein 16.4 g
+Carbohydrates 38.3 g
+Fiber 6.5 g
+Fat 24.5 g
+Cholesterol 0 mg
+Sodium 14.7 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/egg-paratha-42333r</t>
+  </si>
+  <si>
+    <t>Recipe# 7468</t>
+  </si>
+  <si>
+    <t>Fenugreek and Mushroom Brown Rice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 cups finely chopped fenugreek (methi) leaves    </t>
+  </si>
+  <si>
+    <t>, Heat the oil in a pressure cooker, add the green chillies, ginger, garlic, and onions and sauté on a medium flame for 2 minutes.
+Add the fenugreek leaves, mushrooms, tomatoes, brinjals, surti papadi seeds,and chilli powder, mix well and cook on a medium flame for 1 to 2 minutes, while stirring occasionally.
+Add the brown rice, 2¼ cups of hot water and salt, mix well and pressure cook for 4 whistles.
+Allow the steam to escape before opening the lid.
+Serve hot garnished with coriander.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per serving
+Energy 151 cal
+Protein 3.9 g
+Carbohydrates 27.6 g
+Fiber 3.3 g
+Fat 2.8 g
+Cholesterol 0 mg
+Sodium 19.9 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/fenugreek-and-mushroom-brown-rice-7468r</t>
+  </si>
+  <si>
+    <t>Recipe# 40899</t>
+  </si>
+  <si>
+    <t>Roasted Mushroom and Coloured Capsicum Salad</t>
+  </si>
+  <si>
+    <t>5 mins</t>
+  </si>
+  <si>
+    <t>, Wash, clean and dry the mushrooms and place them on a baking tray and bake in a pre-heated oven at 200°c (400°f) for 11 minutes or till the mushrooms turn light brown in colour, while turning them once after 6 minutes. Keep aside to cool slightly.
+Once they are slightly cooled, cut the stems of the mushrooms and discard them.
+Cut the mushrooms into cubes and keep aside.
+Pierce the red capsicum with a fork and roast it over an open flame till it turns black from all the sides.
+Cool, wash it in cold water and remove the burnt skin, stem and seeds and discard them. Cut the capsicum into cubes and keep aside.
+Repeat steps 4 and 5 for green and yellow capsicum.
+Combine the mushroom and capsicum cubes in a deep bowl, add the rosemary, thyme, lemon juice and salt and toss well.
+Serve immediately.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per serving
+Energy 29 cal
+Protein 1.7 g
+Carbohydrates 5.2 g
+Fiber 2.2 g
+Fat 0.4 g
+Cholesterol 0 mg
+Sodium 3.7 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/roasted-mushroom-and-coloured-capsicum-salad-40899r</t>
+  </si>
+  <si>
+    <t>Recipe# 22330</t>
+  </si>
+  <si>
+    <t>Mushroom Brown Rice</t>
+  </si>
+  <si>
+    <t>25 mins</t>
+  </si>
+  <si>
+    <t>, For the brown rice
+Wash and soak the brown rice for 2 to 3 hours. Drain and keep aside.
+Boil 4 cups of water in a large vessel, add the rice and lemon grass and cook over a medium flame till the rice is done. Drain and discard the water and lemon grass and keep aside.
+Heat the oil in a non-stick pan, add the spring onions and sauté till they turn translucent.
+Add the capsicum, green chillies and red chilli flakes and sauté for a while.
+Add the cooked brown rice and salt and mix gently. Remove from the flame and keep aside.
+For the sautéed mushrooms
+Heat the oil in a pan, add the spring onion whites and sauté till they turn translucent.
+Add the garlic and capsicum and fry for a minute.
+Add the ground paste, lemon juice and sauté for another minute.
+Mix well and finally add the mushrooms.
+Cook till they are soft and all the water has dried.
+Add the cornflour mixture and coriander and toss gently. Keep aside.
+How to proceed
+Just before serving heat the sautéed mushrooms in a large kadhai, add the rice to it and toss gently.
+Serve hot garnished with spring onion greens.</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/mushroom-brown-rice-22330r</t>
+  </si>
+  <si>
+    <t>Recipe# 41505</t>
+  </si>
+  <si>
+    <t>Minty Quinoa, Ibs Recipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/4 cup finely chopped mint leaves (phudina) leaves    </t>
+  </si>
+  <si>
+    <t>18 mins</t>
+  </si>
+  <si>
+    <t>, For minty quinoa for ibs
+To make minty quinoa heat oil in a deep non-stick pan, add the carrots, celery and green chillies sauté on a medium flame for 2 minutes.
+Add the quinoa, red pumpkin, bayleaves, salt, pepper powder and 2½ cups of water and mix well. Cover with a lid and cook on a slow flame for 15 to 16 minutes, while stirring occasionally.
+Add the mint leaves and mix well.
+Serve minty quinoa immediately.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per serving
+Energy 208 cal
+Protein 7 g
+Carbohydrates 36.7 g
+Fiber 11 g
+Fat 5.5 g
+Cholesterol 0 mg
+Sodium 14.6 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/minty-quinoa-ibs-recipe-41505r</t>
+  </si>
+  <si>
+    <t>Recipe# 41019</t>
+  </si>
+  <si>
+    <t>Oats, Vegetable and Brown Rice Khichdi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2 cup quick cooking rolled oats    </t>
+  </si>
+  <si>
+    <t>, Clean, wash and soak the brown rice in enough water in a deep bowl for 30 minutes. Drain well and keep aside.
+Heat the oil in a pressure cooker, add the onions, garlic paste and ginger paste and sauté on a medium flame for 1 minute.
+Add the french beans, carrot, green peas, chilli powder and garam masala and sauté on a medium flame for 1 minute.
+Add the brown rice, yellow moong dal, oats, coriander and salt, mix well and cook on a medium flame for 2 minutes, while stirring continuously.
+Add 3 cups of hot water, mix well and pressure cook for 7 whistles.
+Allow the steam to escape before opening the lid.
+Serve hot.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per serving
+Energy 300 cal
+Protein 9.1 g
+Carbohydrates 53.2 g
+Fiber 5.5 g
+Fat 5.6 g
+Cholesterol 0 mg
+Sodium 12.1 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/oats-vegetable-and-brown-rice-khichdi-41019r</t>
+  </si>
+  <si>
+    <t>Recipe# 38954</t>
+  </si>
+  <si>
+    <t>Fluffy Egg White Masala Omelette</t>
+  </si>
+  <si>
+    <t>, For the masala vegetables
+In a pan, heat the olive oil and sauté the onions, capsicums , mushrooms, and green chilli for 1 minute. Add the tomatoes and cook again. Keep aside.
+How to proceed
+Beat the egg whites in a electric beater on a slow for 2 to 3 minutes or until the mixture is thick and frothy.
+Heat the olive oil in a 10 inch pan. Add the beaten egg and cook for a few minutes checking with a spatula to see when the bottom of the egg is done. Then add the cooked masala vegetables in the centre of the omelette. Fold the omelette into half and serve hot with a whole wheat toast.
+Sprinkle fresh pepper on top.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per omeleltte
+Energy 394 cal
+Protein 22 g
+Carbohydrates 8.9 g
+Fiber 2.6 g
+Fat 30.3 g
+Cholesterol 0 mg
+Sodium 9.4 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/fluffy-egg-white-masala-omelette-38954r</t>
+  </si>
+  <si>
+    <t>Recipe# 39688</t>
+  </si>
+  <si>
+    <t>Mushroom and Green Capsicum Subzi</t>
+  </si>
+  <si>
+    <t>, Heat the oil in a broad non-stick pan, add the prepared paste and 2 tbsp of water, mix well and cook on a medium flame for 2 minutes, while stirring occasionally.
+Add the capsicum cubes, mushrooms and salt and mix well. Cover with a lid and cook on a medium flame for 6 to 8 minutes, while stirring occasionally.
+Serve immediately.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per serving
+Energy 59 cal
+Protein 2.3 g
+Carbohydrates 7 g
+Fiber 1.9 g
+Fat 3 g
+Cholesterol 0 mg
+Sodium 4.9 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/mushroom-and-green-capsicum-subzi-39688r</t>
+  </si>
+  <si>
+    <t>Recipe# 1706</t>
+  </si>
+  <si>
+    <t>Dal and Vegetable Idli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2 cup toovar (arhar) dal    1/4 cup yellow moong dal (split yellow gram)    1/2 cup chana dal (split bengal gram)    1 cup chopped fenugreek leaves (methi)    2 cups chopped coriander (dhania)    1/4 cup boiled green peas    </t>
+  </si>
+  <si>
+    <t>0 mins</t>
+  </si>
+  <si>
+    <t>, For dal and vegetable idli
+To make dal and vegetable idli, wash and soak the dals together at least 3 hours.
+Drain, add water and grind to a smooth paste.
+Add the fenugreek, coriander, green peas, coconut, green chillies, onion, carrot and salt and mix well.
+Gradually add water as required to make a thick batter. We added a total of 3/4th cup water.
+Just before steaming, add fruit salt and 1 tbsp of water to the batter and mix gently.
+Pour into greased idli moulds and steam for 10 to 12 minutes till done.
+Serve the dal and vegetable idli hot with sambhar and coconut chutney.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per idli
+Energy 49 cal
+Protein 2.8 g
+Carbohydrates 7.5 g
+Fiber 2 g
+Fat 0.9 g
+Cholesterol 0 mg
+Sodium 9.2 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/dal-and-vegetable-idli-1706r</t>
+  </si>
+  <si>
+    <t>Recipe# 6210</t>
+  </si>
+  <si>
+    <t>Papaya Coconut Drink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 cup papaya cubes    </t>
+  </si>
+  <si>
+    <t>, For papaya coconut drink
+To make papaya coconut drink, combine the papaya cubes, coconut meat, coconut water and ice cubes in a mixer jar and blend well till smooth.
+Serve the papaya coconut drinkimmediately.
+Handy tip:
+This recipe doesn’t turn out good in a juicer (hopper) because the texture of papaya is very soft.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per glass
+Energy 61 cal
+Protein 1.3 g
+Carbohydrates 11 g
+Fiber 9 g
+Fat 1.4 g
+Cholesterol 0 mg
+Sodium 4.2 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/papaya-coconut-drink-6210r</t>
   </si>
   <si>
     <t xml:space="preserve">1/2 cup chawli (cow pea / lobhia) , soaked overnight and drained    salt to taste    1 tbsp coconut oil or oil    1/2 cup finely chopped onions    1 cup fresh tomato pulp    1/2 tsp dried fenugreek leaves (kasuri methi)    1/4 tsp turmeric powder (haldi)    3/4 cup chopped mint leaves (phudina) , washed and drained    1 tsp roughly chopped ginger (adrak)    2 tsp roughly chopped green chillies    1/2 tsp lemon juice    </t>
@@ -210,9 +580,6 @@
     <t xml:space="preserve">3/4 cup toovar (arhar) dal    1/4 cup chana dal (split bengal gram)    1 cup chopped tomatoes    2 cups bottle gourd (doodhi / lauki) , cut into big pieces    1/4 tsp turmeric powder (haldi)    1 tsp cumin seeds (jeera)    1/2 tsp chopped garlic (lehsun)    1 tsp chopped green chillies    1 tsp grated ginger (adrak)    3/4 cup sliced onions    2 tsp oil    salt to taste    2 tbsp chopped coriander (dhania)    </t>
   </si>
   <si>
-    <t>25 mins</t>
-  </si>
-  <si>
     <t>, For dal moghlai
 To make dal moghlai,clean, wash and soak the dals for about 30 minutes. Drain.
 Add the tomatoes, bottle gourd, turmeric powder, salt and 3 cups of water and pressure cook till the dals are tender.
@@ -242,9 +609,6 @@
   </si>
   <si>
     <t xml:space="preserve">1 cup moong (whole green gram) , washed and drained    salt to taste    1/4 tsp turmeric powder (haldi)    </t>
-  </si>
-  <si>
-    <t>1 mins</t>
   </si>
   <si>
     <t>, For moong sprouts
@@ -300,67 +664,12 @@
     <t>https://www.tarladalal.com/oats-moong-dal-tikki-35288r</t>
   </si>
   <si>
-    <t>Recipe# 42296</t>
-  </si>
-  <si>
-    <t>Quinoa Avocado Veg Healthy Office Salad</t>
-  </si>
-  <si>
     <t xml:space="preserve">1/4 cup cooked quinoa    1/2 cup riped avocado cubes    1/2 cup chopped zucchini    1/2 cup coloured capsicum cubes    1/4 cup mushroom (khumbh) cubes    1/4 cup cherry tomato halves    1 cup iceberg lettuce , torn into pieces    1 tbsp alfalfa sprouts    1 tsp olive oil    sea salt (khada namak) to taste    1 tbsp olive oil    1 tsp lemon juice    1/4 tsp grated garlic (lehsun)    sea salt (khada namak) to taste    </t>
   </si>
   <si>
-    <t>3 mins</t>
-  </si>
-  <si>
-    <t>, Heat the olive oil in a griller pan or a broad non-stick pan, add the zucchini and sauté on a medium flame for 1 minute.
-Add the coloured capsicum and sauté on a medium flame for 1 minute.
-Add the mushroom and little sea salt and sauté on a medium flame for 1 minute.
-Cool put in a lunch box, along with other ingredients. It can be taken to work with a dressing in a separate small container.
-Just before eating, mix the dressing and toss well. Eat immediately.</t>
-  </si>
-  <si>
-    <t>Nutrient values (Abbrv) per serving
-Energy 459 cal
-Protein 7.7 g
-Carbohydrates 22 g
-Fiber 6.9 g
-Fat 38.9 g
-Cholesterol 0 mg
-Sodium 60.1 mg</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/quinoa-avocado-veg-healthy-office-salad-42296r</t>
-  </si>
-  <si>
-    <t>Recipe# 39929</t>
-  </si>
-  <si>
-    <t>Brown Rice ( Pressure Cooker Method)</t>
-  </si>
-  <si>
     <t xml:space="preserve">3/4 cup brown rice    salt to taste    </t>
   </si>
   <si>
-    <t>, How to cook brown rice
-To cook brown rice, soak the brown rice in enough water for 30 minutes and drain well.
-Combine the brown rice along with 2 cups of water in a pressure cooker and pressure cook for 7 whistles.
-Allow the steam to escape before opening the lid.
-Separate each grain of the brown rice lightly with a fork. Use as required.</t>
-  </si>
-  <si>
-    <t>Nutrient values (Abbrv) per cup
-Energy 211 cal
-Protein 4.4 g
-Carbohydrates 44.4 g
-Fiber 2 g
-Fat 1.6 g
-Cholesterol 0 mg
-Sodium 2.3 mg</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/brown-rice--pressure-cooker-method-39929r</t>
-  </si>
-  <si>
     <t>Recipe# 6229</t>
   </si>
   <si>
@@ -368,9 +677,6 @@
   </si>
   <si>
     <t xml:space="preserve">1 1/2 cups beetroot cubes    1 1/2 cups carrot cubes    2 tbsp chopped parsley    2 tbsp chopped celery (ajmoda)    1/4 tsp black salt (sanchal)    12 ice-cubes    </t>
-  </si>
-  <si>
-    <t>0 mins</t>
   </si>
   <si>
     <t>, Beetroot juice in blender
@@ -426,33 +732,7 @@
     <t>https://www.tarladalal.com/masoor-dal-easy-masoor-dal-recipe-40586r</t>
   </si>
   <si>
-    <t>Recipe# 7468</t>
-  </si>
-  <si>
-    <t>Fenugreek and Mushroom Brown Rice</t>
-  </si>
-  <si>
     <t xml:space="preserve">2 cups finely chopped fenugreek (methi) leaves    1 cup sliced mushrooms (khumbh)    1 cup brown rice    2 tsp oil    2 tsp finely chopped green chillies    1 tsp finely chopped ginger (adrak)    1 tbsp finely chopped garlic (lehsun)    1 cup finely chopped onions    1/2 cup finely chopped tomatoes    1/2 cup brinjal (baingan / eggplant) cubes    1/2 cup surti papdi seeds (fresh vaal seeds)    1/2 tsp chilli powder    salt to taste    2 tbsp finely chopped coriander (dhania)    </t>
-  </si>
-  <si>
-    <t>, Heat the oil in a pressure cooker, add the green chillies, ginger, garlic, and onions and sauté on a medium flame for 2 minutes.
-Add the fenugreek leaves, mushrooms, tomatoes, brinjals, surti papadi seeds,and chilli powder, mix well and cook on a medium flame for 1 to 2 minutes, while stirring occasionally.
-Add the brown rice, 2¼ cups of hot water and salt, mix well and pressure cook for 4 whistles.
-Allow the steam to escape before opening the lid.
-Serve hot garnished with coriander.</t>
-  </si>
-  <si>
-    <t>Nutrient values (Abbrv) per serving
-Energy 151 cal
-Protein 3.9 g
-Carbohydrates 27.6 g
-Fiber 3.3 g
-Fat 2.8 g
-Cholesterol 0 mg
-Sodium 19.9 mg</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/fenugreek-and-mushroom-brown-rice-7468r</t>
   </si>
   <si>
     <t>Recipe# 22173</t>
@@ -535,9 +815,6 @@
     <t xml:space="preserve">1/2 cup yellow moong dal (split yellow gram)    salt to taste    1/2 cup grated carrot    1/2 cup pomegranate (anar)    1/2 cup chopped spring onions    1/4 cup chopped raw mangoes    2 tbsp finely chopped mint leaves (phudina)    2 tbsp finely chopped coriander (dhania)    2 tsp finely chopped green chillies    1 tsp chaat masala    4 tsp lemon juice    </t>
   </si>
   <si>
-    <t>5 mins</t>
-  </si>
-  <si>
     <t>, For moong dal ki chaat
 To make moong dal ki chaat, clean, wash and soak the moong dal in enough water for ½ hour and drain well.
 Combine 3 cups of water, moong dal and salt in a deep non-stick pan and cook it on a medium flame till it is half done, while stirring occasionally. Ensure that each grain of the dal is separate.
@@ -718,36 +995,7 @@
     <t>https://www.tarladalal.com/masoor-dal-recipe-42353r</t>
   </si>
   <si>
-    <t>Recipe# 40899</t>
-  </si>
-  <si>
-    <t>Roasted Mushroom and Coloured Capsicum Salad</t>
-  </si>
-  <si>
     <t xml:space="preserve">2 cups mushrooms (khumbh)    1 medium red capsicum    1 medium green capsicum    1 medium yellow capsicum    1 tsp dried rosemary or dried mixed herbs    1/2 tsp dried thyme    1 1/2 tsp lemon juice    salt to taste    </t>
-  </si>
-  <si>
-    <t>, Wash, clean and dry the mushrooms and place them on a baking tray and bake in a pre-heated oven at 200°c (400°f) for 11 minutes or till the mushrooms turn light brown in colour, while turning them once after 6 minutes. Keep aside to cool slightly.
-Once they are slightly cooled, cut the stems of the mushrooms and discard them.
-Cut the mushrooms into cubes and keep aside.
-Pierce the red capsicum with a fork and roast it over an open flame till it turns black from all the sides.
-Cool, wash it in cold water and remove the burnt skin, stem and seeds and discard them. Cut the capsicum into cubes and keep aside.
-Repeat steps 4 and 5 for green and yellow capsicum.
-Combine the mushroom and capsicum cubes in a deep bowl, add the rosemary, thyme, lemon juice and salt and toss well.
-Serve immediately.</t>
-  </si>
-  <si>
-    <t>Nutrient values (Abbrv) per serving
-Energy 29 cal
-Protein 1.7 g
-Carbohydrates 5.2 g
-Fiber 2.2 g
-Fat 0.4 g
-Cholesterol 0 mg
-Sodium 3.7 mg</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/roasted-mushroom-and-coloured-capsicum-salad-40899r</t>
   </si>
   <si>
     <t>Recipe# 39020</t>
@@ -1032,67 +1280,10 @@
     <t>https://www.tarladalal.com/baked-masala-sev-40377r</t>
   </si>
   <si>
-    <t>Recipe# 41505</t>
-  </si>
-  <si>
-    <t>Minty Quinoa, Ibs Recipe</t>
-  </si>
-  <si>
     <t xml:space="preserve">1/4 cup finely chopped mint leaves (phudina) leaves    1 cup quinoa , washed and drained    2 tsp olive oil    1/2 cup chopped carrot    1/4 cup chopped celery (ajmoda)    1/2 tsp finely chopped green chillies    1/4 cup chopped red pumpkin (bhopla / kaddu)    2 bay leaves (tejpatta)    salt to taste    freshly ground black pepper (kalimirch) to taste    </t>
   </si>
   <si>
-    <t>18 mins</t>
-  </si>
-  <si>
-    <t>, For minty quinoa for ibs
-To make minty quinoa heat oil in a deep non-stick pan, add the carrots, celery and green chillies sauté on a medium flame for 2 minutes.
-Add the quinoa, red pumpkin, bayleaves, salt, pepper powder and 2½ cups of water and mix well. Cover with a lid and cook on a slow flame for 15 to 16 minutes, while stirring occasionally.
-Add the mint leaves and mix well.
-Serve minty quinoa immediately.</t>
-  </si>
-  <si>
-    <t>Nutrient values (Abbrv) per serving
-Energy 208 cal
-Protein 7 g
-Carbohydrates 36.7 g
-Fiber 11 g
-Fat 5.5 g
-Cholesterol 0 mg
-Sodium 14.6 mg</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/minty-quinoa-ibs-recipe-41505r</t>
-  </si>
-  <si>
-    <t>Recipe# 41019</t>
-  </si>
-  <si>
-    <t>Oats, Vegetable and Brown Rice Khichdi</t>
-  </si>
-  <si>
     <t xml:space="preserve">1/2 cup quick cooking rolled oats    3/4 cup brown rice    2 tbsp yellow moong dal (split yellow gram) , washed and drained    2 tsp oil    1/2 cup finely chopped onions    1 tsp garlic (lehsun) paste    1/2 tsp ginger (adrak) paste    1/4 cup chopped french beans    1/4 cup chopped carrot    1/4 cup green peas    1/2 tsp chilli powder    1/2 tsp garam masala    2 tbsp finely chopped coriander (dhania)    salt to taste    </t>
-  </si>
-  <si>
-    <t>, Clean, wash and soak the brown rice in enough water in a deep bowl for 30 minutes. Drain well and keep aside.
-Heat the oil in a pressure cooker, add the onions, garlic paste and ginger paste and sauté on a medium flame for 1 minute.
-Add the french beans, carrot, green peas, chilli powder and garam masala and sauté on a medium flame for 1 minute.
-Add the brown rice, yellow moong dal, oats, coriander and salt, mix well and cook on a medium flame for 2 minutes, while stirring continuously.
-Add 3 cups of hot water, mix well and pressure cook for 7 whistles.
-Allow the steam to escape before opening the lid.
-Serve hot.</t>
-  </si>
-  <si>
-    <t>Nutrient values (Abbrv) per serving
-Energy 300 cal
-Protein 9.1 g
-Carbohydrates 53.2 g
-Fiber 5.5 g
-Fat 5.6 g
-Cholesterol 0 mg
-Sodium 12.1 mg</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/oats-vegetable-and-brown-rice-khichdi-41019r</t>
   </si>
   <si>
     <t>Recipe# 41364</t>
@@ -1301,61 +1492,10 @@
     <t>https://www.tarladalal.com/avocado-dip-avocado-jain-dip-8651r</t>
   </si>
   <si>
-    <t>Recipe# 38954</t>
-  </si>
-  <si>
-    <t>Fluffy Egg White Masala Omelette</t>
-  </si>
-  <si>
     <t xml:space="preserve">3 eggs whites    1 tsp olive oil    salt and freshly ground to taste    1/4 cup finely chopped onions    1/2 cup red and yellow capsicum chopped    1/4 cup finely chopped mushrooms (khumbh)    1/4 cup finely chopped tomatoes    1/2 tsp finely chopped green chillies    1 tsp olive oil    </t>
   </si>
   <si>
-    <t>, For the masala vegetables
-In a pan, heat the olive oil and sauté the onions, capsicums , mushrooms, and green chilli for 1 minute. Add the tomatoes and cook again. Keep aside.
-How to proceed
-Beat the egg whites in a electric beater on a slow for 2 to 3 minutes or until the mixture is thick and frothy.
-Heat the olive oil in a 10 inch pan. Add the beaten egg and cook for a few minutes checking with a spatula to see when the bottom of the egg is done. Then add the cooked masala vegetables in the centre of the omelette. Fold the omelette into half and serve hot with a whole wheat toast.
-Sprinkle fresh pepper on top.</t>
-  </si>
-  <si>
-    <t>Nutrient values (Abbrv) per omeleltte
-Energy 394 cal
-Protein 22 g
-Carbohydrates 8.9 g
-Fiber 2.6 g
-Fat 30.3 g
-Cholesterol 0 mg
-Sodium 9.4 mg</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/fluffy-egg-white-masala-omelette-38954r</t>
-  </si>
-  <si>
-    <t>Recipe# 39688</t>
-  </si>
-  <si>
-    <t>Mushroom and Green Capsicum Subzi</t>
-  </si>
-  <si>
     <t xml:space="preserve">5 cups mushroom (khumbh) halves    1 cup capsicum cubes    2 tsp oil    salt to taste    4 whole dry kashmiri red chillies , broken into pieces    6 garlic (lehsun) cloves    1/2 cup roughly chopped onions    </t>
-  </si>
-  <si>
-    <t>, Heat the oil in a broad non-stick pan, add the prepared paste and 2 tbsp of water, mix well and cook on a medium flame for 2 minutes, while stirring occasionally.
-Add the capsicum cubes, mushrooms and salt and mix well. Cover with a lid and cook on a medium flame for 6 to 8 minutes, while stirring occasionally.
-Serve immediately.</t>
-  </si>
-  <si>
-    <t>Nutrient values (Abbrv) per serving
-Energy 59 cal
-Protein 2.3 g
-Carbohydrates 7 g
-Fiber 1.9 g
-Fat 3 g
-Cholesterol 0 mg
-Sodium 4.9 mg</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/mushroom-and-green-capsicum-subzi-39688r</t>
   </si>
   <si>
     <t>Recipe# 41020</t>
@@ -1394,36 +1534,7 @@
     <t>https://www.tarladalal.com/gavar-aur-masoor-ki-dal-41020r</t>
   </si>
   <si>
-    <t>Recipe# 1706</t>
-  </si>
-  <si>
-    <t>Dal and Vegetable Idli</t>
-  </si>
-  <si>
     <t xml:space="preserve">1/2 cup toovar (arhar) dal    1/4 cup yellow moong dal (split yellow gram)    1/2 cup chana dal (split bengal gram)    1 cup chopped fenugreek leaves (methi)    2 cups chopped coriander (dhania)    1/4 cup boiled green peas    1/4 cup grated coconut    2 tsp chopped green chillies    1/4 cup chopped onions    1/4 cup grated carrot    salt to taste    oil for greasing    </t>
-  </si>
-  <si>
-    <t>, For dal and vegetable idli
-To make dal and vegetable idli, wash and soak the dals together at least 3 hours.
-Drain, add water and grind to a smooth paste.
-Add the fenugreek, coriander, green peas, coconut, green chillies, onion, carrot and salt and mix well.
-Gradually add water as required to make a thick batter. We added a total of 3/4th cup water.
-Just before steaming, add fruit salt and 1 tbsp of water to the batter and mix gently.
-Pour into greased idli moulds and steam for 10 to 12 minutes till done.
-Serve the dal and vegetable idli hot with sambhar and coconut chutney.</t>
-  </si>
-  <si>
-    <t>Nutrient values (Abbrv) per idli
-Energy 49 cal
-Protein 2.8 g
-Carbohydrates 7.5 g
-Fiber 2 g
-Fat 0.9 g
-Cholesterol 0 mg
-Sodium 9.2 mg</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/dal-and-vegetable-idli-1706r</t>
   </si>
   <si>
     <t>Recipe# 40134</t>
@@ -1571,33 +1682,7 @@
     <t>https://www.tarladalal.com/chawli-rajma-and-chick-pea-healthy-salad-379r</t>
   </si>
   <si>
-    <t>Recipe# 6210</t>
-  </si>
-  <si>
-    <t>Papaya Coconut Drink</t>
-  </si>
-  <si>
     <t xml:space="preserve">1 cup papaya cubes    1/4 cup coconut meat (nariyal ki malai)    3/4 cup chilled coconut water (nariyal ka pani)    10 to 12 ice-cubes    </t>
-  </si>
-  <si>
-    <t>, For papaya coconut drink
-To make papaya coconut drink, combine the papaya cubes, coconut meat, coconut water and ice cubes in a mixer jar and blend well till smooth.
-Serve the papaya coconut drinkimmediately.
-Handy tip:
-This recipe doesn’t turn out good in a juicer (hopper) because the texture of papaya is very soft.</t>
-  </si>
-  <si>
-    <t>Nutrient values (Abbrv) per glass
-Energy 61 cal
-Protein 1.3 g
-Carbohydrates 11 g
-Fiber 9 g
-Fat 1.4 g
-Cholesterol 0 mg
-Sodium 4.2 mg</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/papaya-coconut-drink-6210r</t>
   </si>
   <si>
     <t>Recipe# 3600</t>
@@ -1697,7 +1782,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1803,6 +1888,426 @@
       </c>
       <c r="K3" t="s" s="0">
         <v>26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K6" t="s" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K7" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K8" t="s" s="0">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K9" t="s" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="J10" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K10" t="s" s="0">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="J11" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K11" t="s" s="0">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="J12" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K12" t="s" s="0">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="I13" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="J13" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K13" t="s" s="0">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="H14" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="I14" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="J14" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K14" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="F15" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="G15" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="H15" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="I15" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="J15" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K15" t="s" s="0">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1864,7 +2369,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s" s="0">
         <v>13</v>
@@ -1887,10 +2392,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>2</v>
@@ -1899,33 +2404,33 @@
         <v>3</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>33</v>
+        <v>104</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="J3" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>35</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>2</v>
@@ -1934,25 +2439,25 @@
         <v>3</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>38</v>
+        <v>109</v>
       </c>
       <c r="F4" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="J4" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>42</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5">
@@ -1969,7 +2474,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>43</v>
+        <v>114</v>
       </c>
       <c r="F5" t="s" s="0">
         <v>22</v>
@@ -1992,10 +2497,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>2</v>
@@ -2004,33 +2509,33 @@
         <v>3</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="F6" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="J6" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K6" t="s" s="0">
-        <v>50</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>52</v>
+        <v>122</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>2</v>
@@ -2039,33 +2544,33 @@
         <v>3</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s" s="0">
         <v>13</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>55</v>
+        <v>124</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="J7" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K7" t="s" s="0">
-        <v>57</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>59</v>
+        <v>128</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>2</v>
@@ -2074,33 +2579,33 @@
         <v>3</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>60</v>
+        <v>129</v>
       </c>
       <c r="F8" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>61</v>
+        <v>130</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="J8" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K8" t="s" s="0">
-        <v>63</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>2</v>
@@ -2109,33 +2614,33 @@
         <v>3</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>66</v>
+        <v>133</v>
       </c>
       <c r="F9" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="J9" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K9" t="s" s="0">
-        <v>70</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>2</v>
@@ -2144,33 +2649,33 @@
         <v>3</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>73</v>
+        <v>134</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s" s="0">
         <v>23</v>
       </c>
       <c r="H10" t="s" s="0">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="J10" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K10" t="s" s="0">
-        <v>76</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>77</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>2</v>
@@ -2179,33 +2684,33 @@
         <v>3</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>79</v>
+        <v>137</v>
       </c>
       <c r="F11" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H11" t="s" s="0">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="I11" t="s" s="0">
-        <v>82</v>
+        <v>139</v>
       </c>
       <c r="J11" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K11" t="s" s="0">
-        <v>83</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>84</v>
+        <v>141</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>85</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s" s="0">
         <v>2</v>
@@ -2214,7 +2719,7 @@
         <v>3</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>86</v>
+        <v>143</v>
       </c>
       <c r="F12" t="s" s="0">
         <v>13</v>
@@ -2223,24 +2728,24 @@
         <v>23</v>
       </c>
       <c r="H12" t="s" s="0">
-        <v>87</v>
+        <v>144</v>
       </c>
       <c r="I12" t="s" s="0">
-        <v>88</v>
+        <v>145</v>
       </c>
       <c r="J12" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K12" t="s" s="0">
-        <v>89</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s" s="0">
         <v>2</v>
@@ -2249,7 +2754,7 @@
         <v>3</v>
       </c>
       <c r="E13" t="s" s="0">
-        <v>92</v>
+        <v>147</v>
       </c>
       <c r="F13" t="s" s="0">
         <v>23</v>
@@ -2258,24 +2763,24 @@
         <v>23</v>
       </c>
       <c r="H13" t="s" s="0">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="I13" t="s" s="0">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="J13" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K13" t="s" s="0">
-        <v>95</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>96</v>
+        <v>148</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="C14" t="s" s="0">
         <v>2</v>
@@ -2284,33 +2789,33 @@
         <v>3</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="F14" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G14" t="s" s="0">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="H14" t="s" s="0">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="I14" t="s" s="0">
-        <v>101</v>
+        <v>153</v>
       </c>
       <c r="J14" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K14" t="s" s="0">
-        <v>102</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>103</v>
+        <v>155</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>104</v>
+        <v>156</v>
       </c>
       <c r="C15" t="s" s="0">
         <v>2</v>
@@ -2319,33 +2824,33 @@
         <v>3</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>105</v>
+        <v>157</v>
       </c>
       <c r="F15" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G15" t="s" s="0">
-        <v>106</v>
+        <v>158</v>
       </c>
       <c r="H15" t="s" s="0">
-        <v>107</v>
+        <v>159</v>
       </c>
       <c r="I15" t="s" s="0">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="J15" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K15" t="s" s="0">
-        <v>109</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>110</v>
+        <v>162</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>111</v>
+        <v>163</v>
       </c>
       <c r="C16" t="s" s="0">
         <v>2</v>
@@ -2354,33 +2859,33 @@
         <v>3</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>112</v>
+        <v>164</v>
       </c>
       <c r="F16" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="H16" t="s" s="0">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="I16" t="s" s="0">
-        <v>115</v>
+        <v>166</v>
       </c>
       <c r="J16" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>116</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>117</v>
+        <v>168</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>118</v>
+        <v>169</v>
       </c>
       <c r="C17" t="s" s="0">
         <v>2</v>
@@ -2389,33 +2894,33 @@
         <v>3</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>119</v>
+        <v>170</v>
       </c>
       <c r="F17" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G17" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H17" t="s" s="0">
-        <v>120</v>
+        <v>171</v>
       </c>
       <c r="I17" t="s" s="0">
-        <v>121</v>
+        <v>172</v>
       </c>
       <c r="J17" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K17" t="s" s="0">
-        <v>122</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>123</v>
+        <v>174</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>124</v>
+        <v>175</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>2</v>
@@ -2424,33 +2929,33 @@
         <v>3</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="F18" t="s" s="0">
-        <v>126</v>
+        <v>177</v>
       </c>
       <c r="G18" t="s" s="0">
         <v>13</v>
       </c>
       <c r="H18" t="s" s="0">
-        <v>127</v>
+        <v>178</v>
       </c>
       <c r="I18" t="s" s="0">
-        <v>128</v>
+        <v>179</v>
       </c>
       <c r="J18" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K18" t="s" s="0">
-        <v>129</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>130</v>
+        <v>181</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>131</v>
+        <v>182</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>2</v>
@@ -2459,33 +2964,33 @@
         <v>3</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>132</v>
+        <v>183</v>
       </c>
       <c r="F19" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G19" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H19" t="s" s="0">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="I19" t="s" s="0">
-        <v>134</v>
+        <v>185</v>
       </c>
       <c r="J19" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K19" t="s" s="0">
-        <v>135</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>136</v>
+        <v>187</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>137</v>
+        <v>188</v>
       </c>
       <c r="C20" t="s" s="0">
         <v>2</v>
@@ -2494,33 +2999,33 @@
         <v>3</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>138</v>
+        <v>189</v>
       </c>
       <c r="F20" t="s" s="0">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="G20" t="s" s="0">
-        <v>139</v>
+        <v>190</v>
       </c>
       <c r="H20" t="s" s="0">
-        <v>140</v>
+        <v>191</v>
       </c>
       <c r="I20" t="s" s="0">
-        <v>141</v>
+        <v>192</v>
       </c>
       <c r="J20" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K20" t="s" s="0">
-        <v>142</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>143</v>
+        <v>194</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="C21" t="s" s="0">
         <v>2</v>
@@ -2529,7 +3034,7 @@
         <v>3</v>
       </c>
       <c r="E21" t="s" s="0">
-        <v>145</v>
+        <v>196</v>
       </c>
       <c r="F21" t="s" s="0">
         <v>22</v>
@@ -2538,24 +3043,24 @@
         <v>23</v>
       </c>
       <c r="H21" t="s" s="0">
-        <v>146</v>
+        <v>197</v>
       </c>
       <c r="I21" t="s" s="0">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="J21" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K21" t="s" s="0">
-        <v>148</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>149</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>150</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s" s="0">
         <v>2</v>
@@ -2564,33 +3069,33 @@
         <v>3</v>
       </c>
       <c r="E22" t="s" s="0">
-        <v>151</v>
+        <v>200</v>
       </c>
       <c r="F22" t="s" s="0">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="G22" t="s" s="0">
         <v>13</v>
       </c>
       <c r="H22" t="s" s="0">
-        <v>152</v>
+        <v>54</v>
       </c>
       <c r="I22" t="s" s="0">
-        <v>153</v>
+        <v>55</v>
       </c>
       <c r="J22" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K22" t="s" s="0">
-        <v>154</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>155</v>
+        <v>201</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>156</v>
+        <v>202</v>
       </c>
       <c r="C23" t="s" s="0">
         <v>2</v>
@@ -2599,33 +3104,33 @@
         <v>3</v>
       </c>
       <c r="E23" t="s" s="0">
-        <v>157</v>
+        <v>203</v>
       </c>
       <c r="F23" t="s" s="0">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="G23" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H23" t="s" s="0">
-        <v>158</v>
+        <v>204</v>
       </c>
       <c r="I23" t="s" s="0">
-        <v>159</v>
+        <v>205</v>
       </c>
       <c r="J23" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K23" t="s" s="0">
-        <v>160</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>161</v>
+        <v>207</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>162</v>
+        <v>208</v>
       </c>
       <c r="C24" t="s" s="0">
         <v>2</v>
@@ -2634,33 +3139,33 @@
         <v>3</v>
       </c>
       <c r="E24" t="s" s="0">
-        <v>163</v>
+        <v>209</v>
       </c>
       <c r="F24" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G24" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H24" t="s" s="0">
-        <v>164</v>
+        <v>210</v>
       </c>
       <c r="I24" t="s" s="0">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="J24" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K24" t="s" s="0">
-        <v>166</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>167</v>
+        <v>213</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>168</v>
+        <v>214</v>
       </c>
       <c r="C25" t="s" s="0">
         <v>2</v>
@@ -2669,33 +3174,33 @@
         <v>3</v>
       </c>
       <c r="E25" t="s" s="0">
-        <v>169</v>
+        <v>215</v>
       </c>
       <c r="F25" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G25" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H25" t="s" s="0">
-        <v>170</v>
+        <v>216</v>
       </c>
       <c r="I25" t="s" s="0">
-        <v>171</v>
+        <v>217</v>
       </c>
       <c r="J25" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K25" t="s" s="0">
-        <v>172</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>173</v>
+        <v>219</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="C26" t="s" s="0">
         <v>2</v>
@@ -2704,33 +3209,33 @@
         <v>3</v>
       </c>
       <c r="E26" t="s" s="0">
-        <v>175</v>
+        <v>221</v>
       </c>
       <c r="F26" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G26" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H26" t="s" s="0">
-        <v>176</v>
+        <v>222</v>
       </c>
       <c r="I26" t="s" s="0">
-        <v>177</v>
+        <v>223</v>
       </c>
       <c r="J26" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K26" t="s" s="0">
-        <v>178</v>
+        <v>224</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>179</v>
+        <v>225</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>180</v>
+        <v>226</v>
       </c>
       <c r="C27" t="s" s="0">
         <v>2</v>
@@ -2739,7 +3244,7 @@
         <v>3</v>
       </c>
       <c r="E27" t="s" s="0">
-        <v>181</v>
+        <v>227</v>
       </c>
       <c r="F27" t="s" s="0">
         <v>22</v>
@@ -2748,24 +3253,24 @@
         <v>22</v>
       </c>
       <c r="H27" t="s" s="0">
-        <v>182</v>
+        <v>228</v>
       </c>
       <c r="I27" t="s" s="0">
-        <v>183</v>
+        <v>229</v>
       </c>
       <c r="J27" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K27" t="s" s="0">
-        <v>184</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>186</v>
+        <v>232</v>
       </c>
       <c r="C28" t="s" s="0">
         <v>2</v>
@@ -2774,7 +3279,7 @@
         <v>3</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>187</v>
+        <v>233</v>
       </c>
       <c r="F28" t="s" s="0">
         <v>13</v>
@@ -2783,24 +3288,24 @@
         <v>13</v>
       </c>
       <c r="H28" t="s" s="0">
-        <v>188</v>
+        <v>234</v>
       </c>
       <c r="I28" t="s" s="0">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="J28" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K28" t="s" s="0">
-        <v>190</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>191</v>
+        <v>237</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>192</v>
+        <v>238</v>
       </c>
       <c r="C29" t="s" s="0">
         <v>2</v>
@@ -2809,7 +3314,7 @@
         <v>3</v>
       </c>
       <c r="E29" t="s" s="0">
-        <v>193</v>
+        <v>239</v>
       </c>
       <c r="F29" t="s" s="0">
         <v>22</v>
@@ -2818,24 +3323,24 @@
         <v>13</v>
       </c>
       <c r="H29" t="s" s="0">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="I29" t="s" s="0">
-        <v>195</v>
+        <v>241</v>
       </c>
       <c r="J29" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K29" t="s" s="0">
-        <v>196</v>
+        <v>242</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>197</v>
+        <v>243</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>198</v>
+        <v>244</v>
       </c>
       <c r="C30" t="s" s="0">
         <v>2</v>
@@ -2844,7 +3349,7 @@
         <v>3</v>
       </c>
       <c r="E30" t="s" s="0">
-        <v>199</v>
+        <v>245</v>
       </c>
       <c r="F30" t="s" s="0">
         <v>22</v>
@@ -2853,24 +3358,24 @@
         <v>13</v>
       </c>
       <c r="H30" t="s" s="0">
-        <v>200</v>
+        <v>246</v>
       </c>
       <c r="I30" t="s" s="0">
-        <v>201</v>
+        <v>247</v>
       </c>
       <c r="J30" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K30" t="s" s="0">
-        <v>202</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>203</v>
+        <v>249</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>204</v>
+        <v>250</v>
       </c>
       <c r="C31" t="s" s="0">
         <v>2</v>
@@ -2879,33 +3384,33 @@
         <v>3</v>
       </c>
       <c r="E31" t="s" s="0">
-        <v>205</v>
+        <v>251</v>
       </c>
       <c r="F31" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G31" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H31" t="s" s="0">
-        <v>206</v>
+        <v>252</v>
       </c>
       <c r="I31" t="s" s="0">
-        <v>207</v>
+        <v>253</v>
       </c>
       <c r="J31" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K31" t="s" s="0">
-        <v>208</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>209</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>210</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s" s="0">
         <v>2</v>
@@ -2914,33 +3419,33 @@
         <v>3</v>
       </c>
       <c r="E32" t="s" s="0">
-        <v>211</v>
+        <v>255</v>
       </c>
       <c r="F32" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G32" t="s" s="0">
-        <v>212</v>
+        <v>65</v>
       </c>
       <c r="H32" t="s" s="0">
-        <v>213</v>
+        <v>66</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>214</v>
+        <v>67</v>
       </c>
       <c r="J32" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K32" t="s" s="0">
-        <v>215</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>216</v>
+        <v>69</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>217</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s" s="0">
         <v>2</v>
@@ -2949,33 +3454,33 @@
         <v>3</v>
       </c>
       <c r="E33" t="s" s="0">
-        <v>218</v>
+        <v>256</v>
       </c>
       <c r="F33" t="s" s="0">
         <v>23</v>
       </c>
       <c r="G33" t="s" s="0">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="H33" t="s" s="0">
-        <v>219</v>
+        <v>72</v>
       </c>
       <c r="I33" t="s" s="0">
-        <v>220</v>
+        <v>73</v>
       </c>
       <c r="J33" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K33" t="s" s="0">
-        <v>221</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>222</v>
+        <v>257</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>223</v>
+        <v>258</v>
       </c>
       <c r="C34" t="s" s="0">
         <v>2</v>
@@ -2984,33 +3489,33 @@
         <v>3</v>
       </c>
       <c r="E34" t="s" s="0">
-        <v>224</v>
+        <v>259</v>
       </c>
       <c r="F34" t="s" s="0">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="G34" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H34" t="s" s="0">
-        <v>225</v>
+        <v>260</v>
       </c>
       <c r="I34" t="s" s="0">
-        <v>226</v>
+        <v>261</v>
       </c>
       <c r="J34" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K34" t="s" s="0">
-        <v>227</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>228</v>
+        <v>263</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>229</v>
+        <v>264</v>
       </c>
       <c r="C35" t="s" s="0">
         <v>2</v>
@@ -3019,33 +3524,33 @@
         <v>3</v>
       </c>
       <c r="E35" t="s" s="0">
-        <v>230</v>
+        <v>265</v>
       </c>
       <c r="F35" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G35" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H35" t="s" s="0">
-        <v>231</v>
+        <v>266</v>
       </c>
       <c r="I35" t="s" s="0">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="J35" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K35" t="s" s="0">
-        <v>233</v>
+        <v>268</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>234</v>
+        <v>269</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>235</v>
+        <v>270</v>
       </c>
       <c r="C36" t="s" s="0">
         <v>2</v>
@@ -3054,33 +3559,33 @@
         <v>3</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>236</v>
+        <v>271</v>
       </c>
       <c r="F36" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G36" t="s" s="0">
-        <v>237</v>
+        <v>272</v>
       </c>
       <c r="H36" t="s" s="0">
-        <v>238</v>
+        <v>273</v>
       </c>
       <c r="I36" t="s" s="0">
-        <v>239</v>
+        <v>274</v>
       </c>
       <c r="J36" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K36" t="s" s="0">
-        <v>240</v>
+        <v>275</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>241</v>
+        <v>276</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>242</v>
+        <v>277</v>
       </c>
       <c r="C37" t="s" s="0">
         <v>2</v>
@@ -3089,33 +3594,33 @@
         <v>3</v>
       </c>
       <c r="E37" t="s" s="0">
-        <v>243</v>
+        <v>278</v>
       </c>
       <c r="F37" t="s" s="0">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="G37" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H37" t="s" s="0">
-        <v>244</v>
+        <v>279</v>
       </c>
       <c r="I37" t="s" s="0">
-        <v>245</v>
+        <v>280</v>
       </c>
       <c r="J37" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K37" t="s" s="0">
-        <v>246</v>
+        <v>281</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>247</v>
+        <v>282</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>248</v>
+        <v>283</v>
       </c>
       <c r="C38" t="s" s="0">
         <v>2</v>
@@ -3124,33 +3629,33 @@
         <v>3</v>
       </c>
       <c r="E38" t="s" s="0">
-        <v>249</v>
+        <v>284</v>
       </c>
       <c r="F38" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G38" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H38" t="s" s="0">
-        <v>250</v>
+        <v>285</v>
       </c>
       <c r="I38" t="s" s="0">
-        <v>251</v>
+        <v>286</v>
       </c>
       <c r="J38" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K38" t="s" s="0">
-        <v>252</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>253</v>
+        <v>288</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>254</v>
+        <v>289</v>
       </c>
       <c r="C39" t="s" s="0">
         <v>2</v>
@@ -3159,33 +3664,33 @@
         <v>3</v>
       </c>
       <c r="E39" t="s" s="0">
-        <v>255</v>
+        <v>290</v>
       </c>
       <c r="F39" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G39" t="s" s="0">
-        <v>139</v>
+        <v>190</v>
       </c>
       <c r="H39" t="s" s="0">
-        <v>256</v>
+        <v>291</v>
       </c>
       <c r="I39" t="s" s="0">
-        <v>257</v>
+        <v>292</v>
       </c>
       <c r="J39" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K39" t="s" s="0">
-        <v>258</v>
+        <v>293</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>259</v>
+        <v>294</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>260</v>
+        <v>295</v>
       </c>
       <c r="C40" t="s" s="0">
         <v>2</v>
@@ -3194,33 +3699,33 @@
         <v>3</v>
       </c>
       <c r="E40" t="s" s="0">
-        <v>261</v>
+        <v>296</v>
       </c>
       <c r="F40" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G40" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H40" t="s" s="0">
-        <v>262</v>
+        <v>297</v>
       </c>
       <c r="I40" t="s" s="0">
-        <v>263</v>
+        <v>298</v>
       </c>
       <c r="J40" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K40" t="s" s="0">
-        <v>264</v>
+        <v>299</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>265</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>266</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s" s="0">
         <v>2</v>
@@ -3229,33 +3734,33 @@
         <v>3</v>
       </c>
       <c r="E41" t="s" s="0">
-        <v>267</v>
+        <v>300</v>
       </c>
       <c r="F41" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G41" t="s" s="0">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="H41" t="s" s="0">
-        <v>268</v>
+        <v>77</v>
       </c>
       <c r="I41" t="s" s="0">
-        <v>269</v>
+        <v>78</v>
       </c>
       <c r="J41" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K41" t="s" s="0">
-        <v>270</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>271</v>
+        <v>80</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>272</v>
+        <v>81</v>
       </c>
       <c r="C42" t="s" s="0">
         <v>2</v>
@@ -3264,7 +3769,7 @@
         <v>3</v>
       </c>
       <c r="E42" t="s" s="0">
-        <v>273</v>
+        <v>301</v>
       </c>
       <c r="F42" t="s" s="0">
         <v>13</v>
@@ -3273,24 +3778,24 @@
         <v>22</v>
       </c>
       <c r="H42" t="s" s="0">
-        <v>274</v>
+        <v>82</v>
       </c>
       <c r="I42" t="s" s="0">
-        <v>275</v>
+        <v>83</v>
       </c>
       <c r="J42" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K42" t="s" s="0">
-        <v>276</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>277</v>
+        <v>302</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>278</v>
+        <v>303</v>
       </c>
       <c r="C43" t="s" s="0">
         <v>2</v>
@@ -3299,33 +3804,33 @@
         <v>3</v>
       </c>
       <c r="E43" t="s" s="0">
-        <v>279</v>
+        <v>304</v>
       </c>
       <c r="F43" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G43" t="s" s="0">
-        <v>280</v>
+        <v>305</v>
       </c>
       <c r="H43" t="s" s="0">
-        <v>281</v>
+        <v>306</v>
       </c>
       <c r="I43" t="s" s="0">
-        <v>282</v>
+        <v>307</v>
       </c>
       <c r="J43" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K43" t="s" s="0">
-        <v>283</v>
+        <v>308</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>284</v>
+        <v>85</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>285</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s" s="0">
         <v>2</v>
@@ -3334,33 +3839,33 @@
         <v>3</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>286</v>
+        <v>309</v>
       </c>
       <c r="F44" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G44" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H44" t="s" s="0">
-        <v>287</v>
+        <v>89</v>
       </c>
       <c r="I44" t="s" s="0">
-        <v>288</v>
+        <v>90</v>
       </c>
       <c r="J44" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K44" t="s" s="0">
-        <v>289</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c r="C45" t="s" s="0">
         <v>2</v>
@@ -3369,7 +3874,7 @@
         <v>3</v>
       </c>
       <c r="E45" t="s" s="0">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="F45" t="s" s="0">
         <v>13</v>
@@ -3378,24 +3883,24 @@
         <v>22</v>
       </c>
       <c r="H45" t="s" s="0">
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="I45" t="s" s="0">
-        <v>294</v>
+        <v>314</v>
       </c>
       <c r="J45" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K45" t="s" s="0">
-        <v>295</v>
+        <v>315</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="C46" t="s" s="0">
         <v>2</v>
@@ -3404,33 +3909,33 @@
         <v>3</v>
       </c>
       <c r="E46" t="s" s="0">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="F46" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G46" t="s" s="0">
-        <v>280</v>
+        <v>305</v>
       </c>
       <c r="H46" t="s" s="0">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="I46" t="s" s="0">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="J46" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K46" t="s" s="0">
-        <v>301</v>
+        <v>321</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c r="C47" t="s" s="0">
         <v>2</v>
@@ -3439,33 +3944,33 @@
         <v>3</v>
       </c>
       <c r="E47" t="s" s="0">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="F47" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G47" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H47" t="s" s="0">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="I47" t="s" s="0">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="J47" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K47" t="s" s="0">
-        <v>307</v>
+        <v>327</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="C48" t="s" s="0">
         <v>2</v>
@@ -3474,33 +3979,33 @@
         <v>3</v>
       </c>
       <c r="E48" t="s" s="0">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="F48" t="s" s="0">
         <v>23</v>
       </c>
       <c r="G48" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H48" t="s" s="0">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="I48" t="s" s="0">
-        <v>312</v>
+        <v>332</v>
       </c>
       <c r="J48" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K48" t="s" s="0">
-        <v>313</v>
+        <v>333</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="C49" t="s" s="0">
         <v>2</v>
@@ -3509,33 +4014,33 @@
         <v>3</v>
       </c>
       <c r="E49" t="s" s="0">
-        <v>316</v>
+        <v>336</v>
       </c>
       <c r="F49" t="s" s="0">
         <v>22</v>
       </c>
       <c r="G49" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H49" t="s" s="0">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="I49" t="s" s="0">
-        <v>318</v>
+        <v>338</v>
       </c>
       <c r="J49" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K49" t="s" s="0">
-        <v>319</v>
+        <v>339</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>320</v>
+        <v>92</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>321</v>
+        <v>93</v>
       </c>
       <c r="C50" t="s" s="0">
         <v>2</v>
@@ -3544,33 +4049,33 @@
         <v>3</v>
       </c>
       <c r="E50" t="s" s="0">
-        <v>322</v>
+        <v>340</v>
       </c>
       <c r="F50" t="s" s="0">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="G50" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H50" t="s" s="0">
-        <v>323</v>
+        <v>95</v>
       </c>
       <c r="I50" t="s" s="0">
-        <v>324</v>
+        <v>96</v>
       </c>
       <c r="J50" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K50" t="s" s="0">
-        <v>325</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>327</v>
+        <v>342</v>
       </c>
       <c r="C51" t="s" s="0">
         <v>2</v>
@@ -3579,33 +4084,33 @@
         <v>3</v>
       </c>
       <c r="E51" t="s" s="0">
-        <v>328</v>
+        <v>343</v>
       </c>
       <c r="F51" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G51" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H51" t="s" s="0">
-        <v>329</v>
+        <v>344</v>
       </c>
       <c r="I51" t="s" s="0">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="J51" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K51" t="s" s="0">
-        <v>331</v>
+        <v>346</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>332</v>
+        <v>347</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="C52" t="s" s="0">
         <v>2</v>
@@ -3614,25 +4119,25 @@
         <v>3</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>334</v>
+        <v>349</v>
       </c>
       <c r="F52" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G52" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H52" t="s" s="0">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="I52" t="s" s="0">
-        <v>336</v>
+        <v>351</v>
       </c>
       <c r="J52" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K52" t="s" s="0">
-        <v>337</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>